<commit_message>
Added Geofence Debounce Times tests
</commit_message>
<xml_diff>
--- a/TestCoverage.xlsx
+++ b/TestCoverage.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="151">
   <si>
     <t>PollResponse1</t>
   </si>
@@ -474,13 +474,16 @@
   </si>
   <si>
     <t>propget</t>
+  </si>
+  <si>
+    <t>#38</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,6 +510,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -514,7 +525,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -524,6 +535,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
@@ -562,22 +578,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="20% — akcent 6" xfId="3" builtinId="50"/>
-    <cellStyle name="Dane wejściowe" xfId="2" builtinId="20"/>
+  <cellStyles count="5">
+    <cellStyle name="20% — akcent 6" xfId="4" builtinId="50"/>
+    <cellStyle name="Dane wejściowe" xfId="3" builtinId="20"/>
     <cellStyle name="Dobry" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutralny" xfId="2" builtinId="28"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -858,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,7 +1215,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>30</v>
       </c>
@@ -1210,7 +1229,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>32</v>
       </c>
@@ -1224,7 +1243,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>34</v>
       </c>
@@ -1238,7 +1257,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>36</v>
       </c>
@@ -1252,7 +1271,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>38</v>
       </c>
@@ -1266,7 +1285,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
@@ -1280,7 +1299,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>42</v>
       </c>
@@ -1294,7 +1313,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
         <v>101</v>
       </c>
@@ -1302,7 +1321,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
         <v>103</v>
       </c>
@@ -1310,7 +1329,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
         <v>105</v>
       </c>
@@ -1318,7 +1337,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
         <v>107</v>
       </c>
@@ -1326,7 +1345,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>109</v>
       </c>
@@ -1334,7 +1353,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H29" s="1" t="s">
         <v>111</v>
       </c>
@@ -1342,23 +1361,29 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H30" t="s">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H30" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="4" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H31" t="s">
         <v>115</v>
       </c>
       <c r="I31" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H32" s="1" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
HW client disconnected modifications
</commit_message>
<xml_diff>
--- a/TestCoverage.xlsx
+++ b/TestCoverage.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BR\Projektowe\Workspace\swm2m_vms_tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VMSTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -476,10 +476,10 @@
     <t>propget</t>
   </si>
   <si>
-    <t>#39</t>
-  </si>
-  <si>
     <t>no framework functions</t>
+  </si>
+  <si>
+    <t>#39 - workaround done, needs to be testes</t>
   </si>
 </sst>
 </file>
@@ -881,7 +881,7 @@
   <dimension ref="B1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,7 +892,7 @@
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
     <col min="8" max="8" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" customWidth="1"/>
+    <col min="10" max="10" width="42" customWidth="1"/>
     <col min="11" max="11" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1230,7 +1230,7 @@
         <v>88</v>
       </c>
       <c r="J17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -1247,7 +1247,7 @@
         <v>90</v>
       </c>
       <c r="J18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
         <v>92</v>
       </c>
       <c r="J19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -1281,7 +1281,7 @@
         <v>94</v>
       </c>
       <c r="J20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -1298,7 +1298,7 @@
         <v>96</v>
       </c>
       <c r="J21" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -1315,7 +1315,7 @@
         <v>98</v>
       </c>
       <c r="J22" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -1332,7 +1332,7 @@
         <v>100</v>
       </c>
       <c r="J23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -1343,7 +1343,7 @@
         <v>102</v>
       </c>
       <c r="J24" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -1475,10 +1475,10 @@
       </c>
     </row>
     <row r="41" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H41" t="s">
+      <c r="H41" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="1" t="s">
         <v>136</v>
       </c>
     </row>

</xml_diff>